<commit_message>
Added time for 31.1.
</commit_message>
<xml_diff>
--- a/Documents/expenditure_of_time.xlsx
+++ b/Documents/expenditure_of_time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Datamodel, Activity Diagram</t>
+  </si>
+  <si>
+    <t>Enhancement Data Model &amp; Activity Diagram, Technology check "Appguyver, steroids"</t>
+  </si>
+  <si>
+    <t>simple custom quizduell app with steroids-technology</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -539,6 +545,29 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>41670</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>